<commit_message>
changed the fomulars and calculatiosn...nothing else changed ~~
haha
</commit_message>
<xml_diff>
--- a/advanced_stats/testing result.xlsx
+++ b/advanced_stats/testing result.xlsx
@@ -9,11 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3020" yWindow="460" windowWidth="22980" windowHeight="16540" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="460" windowWidth="22980" windowHeight="16540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$47</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$2</definedName>
+  </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -300,7 +304,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -338,8 +342,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -364,6 +374,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -378,7 +394,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -386,11 +402,13 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,6 +564,51 @@
             </a:rPr>
             <a:t>OppOREB/(OppOREB/TmDREB)   </a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>NO</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr lvl="0"/>
@@ -559,7 +622,31 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>OppOREB/(OppOREB + TmDREB)   </a:t>
+            <a:t>OppOREB/(OppOREB + TmDREB)  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Yes</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
@@ -734,6 +821,51 @@
             </a:rPr>
             <a:t>Stops1 + Stops2 </a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>   </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Yes</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr lvl="0"/>
@@ -808,6 +940,30 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>function</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>NO</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="1" baseline="0">
@@ -953,6 +1109,51 @@
             </a:rPr>
             <a:t>TmOREB/(TmOREB+(OppTREB-OppDREB))</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>NO</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr lvl="0"/>
@@ -1027,6 +1228,30 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>function</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Yes</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100" b="1">
@@ -1326,7 +1551,7 @@
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A23" sqref="A23:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1518,24 +1743,24 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="10">
         <v>81.650000000000006</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="10">
         <v>98</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="10">
         <f t="shared" si="1"/>
         <v>16.349999999999994</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="11">
         <f t="shared" si="0"/>
         <v>0.1668367346938775</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="10" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1562,24 +1787,24 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="7">
-        <v>20</v>
-      </c>
-      <c r="C13" s="7">
+      <c r="B13" s="10">
+        <v>0.45939999999999998</v>
+      </c>
+      <c r="C13" s="10">
         <v>0.45900000000000002</v>
       </c>
-      <c r="D13" s="7">
-        <f t="shared" si="1"/>
-        <v>-19.541</v>
-      </c>
-      <c r="E13" s="8">
-        <f t="shared" si="0"/>
-        <v>-42.572984749455337</v>
-      </c>
-      <c r="F13" s="7" t="s">
+      <c r="D13" s="10">
+        <f t="shared" si="1"/>
+        <v>-3.9999999999995595E-4</v>
+      </c>
+      <c r="E13" s="11">
+        <f t="shared" si="0"/>
+        <v>-8.7145969498901078E-4</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1650,46 +1875,46 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="10">
         <v>2.5499999999999998</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="10">
         <v>1.9</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="10">
         <f t="shared" si="1"/>
         <v>-0.64999999999999991</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="11">
         <f t="shared" si="0"/>
         <v>-0.34210526315789469</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="10">
         <v>0.37390000000000001</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="10">
         <v>0.9</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="10">
         <f t="shared" si="1"/>
         <v>0.52610000000000001</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="11">
         <f t="shared" si="0"/>
         <v>0.58455555555555561</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="10" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1988,24 +2213,24 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="7">
-        <v>0.34599999999999997</v>
-      </c>
-      <c r="C33" s="7">
+      <c r="B33" s="10">
+        <v>0.23069999999999999</v>
+      </c>
+      <c r="C33" s="10">
         <v>0.23100000000000001</v>
       </c>
-      <c r="D33" s="7">
-        <f t="shared" si="1"/>
-        <v>-0.11499999999999996</v>
-      </c>
-      <c r="E33" s="8">
-        <f t="shared" si="0"/>
-        <v>-0.49783549783549763</v>
-      </c>
-      <c r="F33" s="7" t="s">
+      <c r="D33" s="10">
+        <f t="shared" si="1"/>
+        <v>3.0000000000002247E-4</v>
+      </c>
+      <c r="E33" s="11">
+        <f t="shared" si="0"/>
+        <v>1.2987012987013958E-3</v>
+      </c>
+      <c r="F33" s="10" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2307,8 +2532,9 @@
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" copies="2"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>